<commit_message>
added new plots for logistic results
</commit_message>
<xml_diff>
--- a/Logistic results.xlsx
+++ b/Logistic results.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="17">
   <si>
     <t>Threshold: .5</t>
   </si>
@@ -96,12 +96,18 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -116,7 +122,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -125,10 +131,20 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -253,37 +269,37 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$B$10:$K$10</c:f>
+              <c:f>Sheet1!$B$10:$L$10</c:f>
               <c:strCache>
-                <c:ptCount val="10"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>Original</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>Upsample of 5 times</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>Upsample of 10 times</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>Upsample of 15 times</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>Upsample of 20 times</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>Upsample of 25 times</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>Upsample of 40 times</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>Upsample of 50 times</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="9">
                   <c:v>Upsample of 75 times</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="10">
                   <c:v>Upsample of 100 times</c:v>
                 </c:pt>
               </c:strCache>
@@ -291,38 +307,38 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$11:$K$11</c:f>
+              <c:f>Sheet1!$B$11:$L$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>0.99720989999999998</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0.99519740000000001</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>0.99243009999999998</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>0.98996019999999996</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>0.98771900000000001</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>0.98586649999999998</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>0.97932580000000002</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>0.97527790000000003</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="9">
                   <c:v>0.96647300000000003</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="10">
                   <c:v>0.9572794</c:v>
                 </c:pt>
               </c:numCache>
@@ -613,37 +629,37 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$B$13:$K$13</c:f>
+              <c:f>Sheet1!$B$13:$L$13</c:f>
               <c:strCache>
-                <c:ptCount val="10"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>Original</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>Upsample of 5 times</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>Upsample of 10 times</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>Upsample of 15 times</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>Upsample of 20 times</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>Upsample of 25 times</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>Upsample of 40 times</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>Upsample of 50 times</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="9">
                   <c:v>Upsample of 75 times</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="10">
                   <c:v>Upsample of 100 times</c:v>
                 </c:pt>
               </c:strCache>
@@ -651,38 +667,38 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$14:$K$14</c:f>
+              <c:f>Sheet1!$B$14:$L$14</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>0.99688969999999999</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0.99732419999999999</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>0.99714130000000001</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>0.99700409999999995</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>0.99682110000000002</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>0.99666100000000002</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>0.99576909999999996</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>0.99499150000000003</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="9">
                   <c:v>0.99288750000000003</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="10">
                   <c:v>0.9908979</c:v>
                 </c:pt>
               </c:numCache>
@@ -875,6 +891,31 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Accuracy With threshold .915</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -948,37 +989,37 @@
           </c:marker>
           <c:xVal>
             <c:strRef>
-              <c:f>Sheet1!$B$13:$K$13</c:f>
+              <c:f>Sheet1!$B$13:$L$13</c:f>
               <c:strCache>
-                <c:ptCount val="10"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>Original</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>Upsample of 5 times</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>Upsample of 10 times</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>Upsample of 15 times</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>Upsample of 20 times</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>Upsample of 25 times</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>Upsample of 40 times</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>Upsample of 50 times</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="9">
                   <c:v>Upsample of 75 times</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="10">
                   <c:v>Upsample of 100 times</c:v>
                 </c:pt>
               </c:strCache>
@@ -986,38 +1027,38 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$B$14:$K$14</c:f>
+              <c:f>Sheet1!$B$14:$L$14</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>0.99688969999999999</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0.99732419999999999</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>0.99714130000000001</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>0.99700409999999995</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>0.99682110000000002</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>0.99666100000000002</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>0.99576909999999996</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>0.99499150000000003</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="9">
                   <c:v>0.99288750000000003</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="10">
                   <c:v>0.9908979</c:v>
                 </c:pt>
               </c:numCache>
@@ -1224,6 +1265,31 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Accuracy with threshold .5</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1297,37 +1363,37 @@
           </c:marker>
           <c:xVal>
             <c:strRef>
-              <c:f>Sheet1!$B$10:$K$10</c:f>
+              <c:f>Sheet1!$B$10:$L$10</c:f>
               <c:strCache>
-                <c:ptCount val="10"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>Original</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>Upsample of 5 times</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>Upsample of 10 times</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>Upsample of 15 times</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>Upsample of 20 times</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>Upsample of 25 times</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>Upsample of 40 times</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>Upsample of 50 times</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="9">
                   <c:v>Upsample of 75 times</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="10">
                   <c:v>Upsample of 100 times</c:v>
                 </c:pt>
               </c:strCache>
@@ -1335,38 +1401,38 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$B$11:$K$11</c:f>
+              <c:f>Sheet1!$B$11:$L$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>0.99720989999999998</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0.99519740000000001</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>0.99243009999999998</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>0.98996019999999996</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>0.98771900000000001</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>0.98586649999999998</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>0.97932580000000002</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>0.97527790000000003</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="9">
                   <c:v>0.96647300000000003</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="10">
                   <c:v>0.9572794</c:v>
                 </c:pt>
               </c:numCache>
@@ -1521,6 +1587,498 @@
         <a:effectLst/>
       </c:spPr>
     </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Logistic</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> regression accuracy</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$B$16</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Threshold: .5</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$A$17:$A$26</c:f>
+              <c:strCache>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>Original</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Upsample of 5 times</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Upsample of 10 times</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Upsample of 15 times</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Upsample of 20 times</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Upsample of 25 times</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Upsample of 40 times</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Upsample of 50 times</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Upsample of 75 times</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Upsample of 100 times</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$17:$B$26</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>0.99720989999999998</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.99519740000000001</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.99243009999999998</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.98996019999999996</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.98771900000000001</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.98586649999999998</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.97932580000000002</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.97527790000000003</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.96647300000000003</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.9572794</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-A8BA-473F-B587-D3E804709CF5}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$C$16</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Threshold: .915</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$A$17:$A$26</c:f>
+              <c:strCache>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>Original</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Upsample of 5 times</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Upsample of 10 times</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Upsample of 15 times</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Upsample of 20 times</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Upsample of 25 times</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Upsample of 40 times</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Upsample of 50 times</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Upsample of 75 times</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Upsample of 100 times</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$C$17:$C$26</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>0.99688969999999999</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.99732419999999999</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.99714130000000001</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.99700409999999995</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.99682110000000002</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.99666100000000002</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.99576909999999996</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.99499150000000003</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.99288750000000003</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.9908979</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-A8BA-473F-B587-D3E804709CF5}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="445555992"/>
+        <c:axId val="445556320"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="445555992"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="445556320"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="445556320"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="1"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="445555992"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
@@ -1718,6 +2276,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
@@ -3737,6 +4335,509 @@
         <a:round/>
       </a:ln>
     </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:valueAxis>
   <cs:wall>
@@ -3761,15 +4862,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>259080</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>83820</xdr:rowOff>
+      <xdr:colOff>60960</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>99060</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>563880</xdr:colOff>
-      <xdr:row>30</xdr:row>
-      <xdr:rowOff>83820</xdr:rowOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>365760</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>99060</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3790,16 +4891,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>426720</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>228600</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>53340</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>17</xdr:col>
-      <xdr:colOff>99060</xdr:colOff>
-      <xdr:row>31</xdr:row>
-      <xdr:rowOff>15240</xdr:rowOff>
+      <xdr:colOff>510540</xdr:colOff>
+      <xdr:row>51</xdr:row>
+      <xdr:rowOff>30480</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3821,15 +4922,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>7620</xdr:colOff>
-      <xdr:row>32</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
+      <xdr:colOff>419100</xdr:colOff>
+      <xdr:row>52</xdr:row>
+      <xdr:rowOff>129540</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>312420</xdr:colOff>
-      <xdr:row>47</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>67</xdr:row>
+      <xdr:rowOff>129540</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3851,15 +4952,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>198120</xdr:colOff>
-      <xdr:row>32</xdr:row>
-      <xdr:rowOff>99060</xdr:rowOff>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>52</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>502920</xdr:colOff>
-      <xdr:row>47</xdr:row>
-      <xdr:rowOff>99060</xdr:rowOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>67</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3873,6 +4974,36 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>53340</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>487680</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>68580</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="9" name="Chart 8"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId5"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -4178,106 +5309,149 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AC14"/>
+  <dimension ref="A1:AB26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1"/>
+    <sheetView tabSelected="1" topLeftCell="A35" workbookViewId="0">
+      <selection activeCell="A16" sqref="A16:C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:29" x14ac:dyDescent="0.3">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A1" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="B1" s="4"/>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
-      <c r="E1" s="4"/>
-      <c r="F1" s="4"/>
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
+      <c r="G1" s="5"/>
     </row>
-    <row r="2" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B2" s="5"/>
-      <c r="C2" s="5"/>
-      <c r="D2" s="5"/>
-      <c r="E2" s="5"/>
-      <c r="F2" s="5"/>
-      <c r="G2" s="5"/>
-      <c r="H2" s="5"/>
+      <c r="B2" s="4"/>
+      <c r="C2" s="4"/>
+      <c r="D2" s="4"/>
+      <c r="E2" s="4"/>
+      <c r="F2" s="4"/>
+      <c r="G2" s="4"/>
+      <c r="H2" s="4"/>
+      <c r="I2" s="4"/>
     </row>
-    <row r="4" spans="1:29" ht="20.399999999999999" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="B3" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" s="6"/>
+      <c r="D3" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="E3" s="8"/>
+      <c r="F3" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="G3" s="7"/>
+      <c r="H3" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="I3" s="8"/>
+      <c r="J3" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="K3" s="7"/>
+      <c r="L3" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="M3" s="9"/>
+      <c r="N3" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="O3" s="7"/>
+      <c r="P3" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q3" s="7"/>
+      <c r="R3" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="S3" s="7"/>
+      <c r="T3" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="U3" s="7"/>
+      <c r="V3" s="8"/>
+      <c r="Y3" s="8"/>
+    </row>
+    <row r="4" spans="1:28" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A4" s="2"/>
       <c r="B4" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="2"/>
+      <c r="C4" s="2" t="s">
+        <v>1</v>
+      </c>
       <c r="D4" s="2" t="s">
         <v>0</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="F4" s="2"/>
+      <c r="F4" s="2" t="s">
+        <v>0</v>
+      </c>
       <c r="G4" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="H4" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="H4" s="2" t="s">
+      <c r="I4" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="I4" s="2"/>
       <c r="J4" s="2" t="s">
         <v>0</v>
       </c>
       <c r="K4" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="L4" s="2"/>
+      <c r="L4" s="2" t="s">
+        <v>0</v>
+      </c>
       <c r="M4" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="N4" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="N4" s="2" t="s">
+      <c r="O4" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="O4" s="2"/>
       <c r="P4" s="2" t="s">
         <v>0</v>
       </c>
       <c r="Q4" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="R4" s="2"/>
+      <c r="R4" s="2" t="s">
+        <v>0</v>
+      </c>
       <c r="S4" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="T4" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="T4" s="2" t="s">
+      <c r="U4" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="U4" s="2"/>
-      <c r="V4" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="W4" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="X4" s="2"/>
-      <c r="Y4" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="Z4" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="AA4" s="2"/>
-      <c r="AB4" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="AC4" s="2" t="s">
-        <v>1</v>
-      </c>
+      <c r="V4" s="2"/>
+      <c r="Y4" s="2"/>
+      <c r="AB4" s="2"/>
     </row>
-    <row r="5" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>2</v>
       </c>
@@ -4293,69 +5467,64 @@
       <c r="E5" s="3">
         <v>0.99732419999999999</v>
       </c>
-      <c r="F5" s="2"/>
+      <c r="F5" s="3">
+        <v>0.99243009999999998</v>
+      </c>
       <c r="G5" s="3">
-        <v>0.99243009999999998</v>
+        <v>0.99714130000000001</v>
       </c>
       <c r="H5" s="3">
-        <v>0.99714130000000001</v>
-      </c>
-      <c r="I5" s="2"/>
+        <v>0.98996019999999996</v>
+      </c>
+      <c r="I5" s="3">
+        <v>0.99700409999999995</v>
+      </c>
       <c r="J5" s="3">
-        <v>0.98996019999999996</v>
+        <v>0.98771900000000001</v>
       </c>
       <c r="K5" s="3">
-        <v>0.99700409999999995</v>
-      </c>
-      <c r="L5" s="2"/>
+        <v>0.99682110000000002</v>
+      </c>
+      <c r="L5" s="3">
+        <v>0.98586649999999998</v>
+      </c>
       <c r="M5" s="3">
-        <v>0.98771900000000001</v>
+        <v>0.99666100000000002</v>
       </c>
       <c r="N5" s="3">
-        <v>0.99682110000000002</v>
-      </c>
-      <c r="O5" s="2"/>
+        <v>0.97932580000000002</v>
+      </c>
+      <c r="O5" s="3">
+        <v>0.99576909999999996</v>
+      </c>
       <c r="P5" s="3">
-        <v>0.98586649999999998</v>
+        <v>0.97527790000000003</v>
       </c>
       <c r="Q5" s="3">
-        <v>0.99666100000000002</v>
-      </c>
-      <c r="R5" s="2"/>
+        <v>0.99499150000000003</v>
+      </c>
+      <c r="R5" s="3">
+        <v>0.96647300000000003</v>
+      </c>
       <c r="S5" s="3">
-        <v>0.97932580000000002</v>
+        <v>0.99288750000000003</v>
       </c>
       <c r="T5" s="3">
-        <v>0.99576909999999996</v>
-      </c>
-      <c r="U5" s="2"/>
-      <c r="V5" s="3">
-        <v>0.97527790000000003</v>
-      </c>
-      <c r="W5" s="3">
-        <v>0.99499150000000003</v>
-      </c>
-      <c r="X5" s="2"/>
-      <c r="Y5" s="3">
-        <v>0.96647300000000003</v>
-      </c>
-      <c r="Z5" s="3">
-        <v>0.99288750000000003</v>
-      </c>
-      <c r="AA5" s="2"/>
-      <c r="AB5" s="3">
         <v>0.9572794</v>
       </c>
-      <c r="AC5" s="3">
+      <c r="U5" s="3">
         <v>0.9908979</v>
       </c>
+      <c r="V5" s="2"/>
+      <c r="Y5" s="2"/>
+      <c r="AB5" s="2"/>
     </row>
-    <row r="9" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A10" s="2"/>
       <c r="B10" s="2" t="s">
         <v>3</v>
@@ -4363,32 +5532,33 @@
       <c r="C10" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D10" s="1" t="s">
+      <c r="D10" s="1"/>
+      <c r="E10" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E10" s="1" t="s">
+      <c r="F10" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="F10" s="1" t="s">
+      <c r="G10" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="G10" s="1" t="s">
+      <c r="H10" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="H10" s="1" t="s">
+      <c r="I10" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="I10" s="1" t="s">
+      <c r="J10" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="J10" s="1" t="s">
+      <c r="K10" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="K10" s="1" t="s">
+      <c r="L10" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>2</v>
       </c>
@@ -4398,37 +5568,38 @@
       <c r="C11" s="3">
         <v>0.99519740000000001</v>
       </c>
-      <c r="D11" s="3">
+      <c r="D11" s="3"/>
+      <c r="E11" s="3">
         <v>0.99243009999999998</v>
       </c>
-      <c r="E11" s="3">
+      <c r="F11" s="3">
         <v>0.98996019999999996</v>
       </c>
-      <c r="F11" s="3">
+      <c r="G11" s="3">
         <v>0.98771900000000001</v>
       </c>
-      <c r="G11" s="3">
+      <c r="H11" s="3">
         <v>0.98586649999999998</v>
       </c>
-      <c r="H11" s="3">
+      <c r="I11" s="3">
         <v>0.97932580000000002</v>
       </c>
-      <c r="I11" s="3">
+      <c r="J11" s="3">
         <v>0.97527790000000003</v>
       </c>
-      <c r="J11" s="1">
+      <c r="K11" s="1">
         <v>0.96647300000000003</v>
       </c>
-      <c r="K11" s="1">
+      <c r="L11" s="1">
         <v>0.9572794</v>
       </c>
     </row>
-    <row r="12" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="13" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A13" s="2"/>
       <c r="B13" s="2" t="s">
         <v>3</v>
@@ -4436,32 +5607,33 @@
       <c r="C13" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D13" s="1" t="s">
+      <c r="D13" s="1"/>
+      <c r="E13" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E13" s="1" t="s">
+      <c r="F13" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="F13" s="1" t="s">
+      <c r="G13" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="G13" s="1" t="s">
+      <c r="H13" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="H13" s="1" t="s">
+      <c r="I13" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="I13" s="1" t="s">
+      <c r="J13" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="J13" s="1" t="s">
+      <c r="K13" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="K13" s="1" t="s">
+      <c r="L13" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
         <v>2</v>
       </c>
@@ -4471,36 +5643,163 @@
       <c r="C14" s="3">
         <v>0.99732419999999999</v>
       </c>
-      <c r="D14" s="3">
+      <c r="D14" s="3"/>
+      <c r="E14" s="3">
         <v>0.99714130000000001</v>
       </c>
-      <c r="E14" s="3">
+      <c r="F14" s="3">
         <v>0.99700409999999995</v>
       </c>
-      <c r="F14" s="3">
+      <c r="G14" s="3">
         <v>0.99682110000000002</v>
       </c>
-      <c r="G14" s="3">
+      <c r="H14" s="3">
         <v>0.99666100000000002</v>
       </c>
-      <c r="H14" s="3">
+      <c r="I14" s="3">
         <v>0.99576909999999996</v>
       </c>
-      <c r="I14" s="3">
+      <c r="J14" s="3">
         <v>0.99499150000000003</v>
       </c>
-      <c r="J14" s="3">
+      <c r="K14" s="3">
         <v>0.99288750000000003</v>
       </c>
-      <c r="K14" s="3">
+      <c r="L14" s="3">
         <v>0.9908979</v>
       </c>
-      <c r="L14" s="1"/>
       <c r="M14" s="1"/>
+      <c r="N14" s="1"/>
+    </row>
+    <row r="16" spans="1:28" ht="20.399999999999999" x14ac:dyDescent="0.3">
+      <c r="B16" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A17" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B17" s="3">
+        <v>0.99720989999999998</v>
+      </c>
+      <c r="C17" s="1">
+        <v>0.99688969999999999</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A18" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B18" s="3">
+        <v>0.99519740000000001</v>
+      </c>
+      <c r="C18" s="3">
+        <v>0.99732419999999999</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A19" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="B19" s="3">
+        <v>0.99243009999999998</v>
+      </c>
+      <c r="C19" s="3">
+        <v>0.99714130000000001</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A20" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B20" s="3">
+        <v>0.98996019999999996</v>
+      </c>
+      <c r="C20" s="3">
+        <v>0.99700409999999995</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A21" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="B21" s="3">
+        <v>0.98771900000000001</v>
+      </c>
+      <c r="C21" s="3">
+        <v>0.99682110000000002</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A22" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B22" s="3">
+        <v>0.98586649999999998</v>
+      </c>
+      <c r="C22" s="3">
+        <v>0.99666100000000002</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A23" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B23" s="3">
+        <v>0.97932580000000002</v>
+      </c>
+      <c r="C23" s="3">
+        <v>0.99576909999999996</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A24" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B24" s="3">
+        <v>0.97527790000000003</v>
+      </c>
+      <c r="C24" s="3">
+        <v>0.99499150000000003</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A25" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B25" s="3">
+        <v>0.96647300000000003</v>
+      </c>
+      <c r="C25" s="3">
+        <v>0.99288750000000003</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A26" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B26" s="3">
+        <v>0.9572794</v>
+      </c>
+      <c r="C26" s="3">
+        <v>0.9908979</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A1:F1"/>
+  <mergeCells count="9">
+    <mergeCell ref="F3:G3"/>
+    <mergeCell ref="J3:K3"/>
+    <mergeCell ref="L3:M3"/>
+    <mergeCell ref="P3:Q3"/>
+    <mergeCell ref="T3:U3"/>
+    <mergeCell ref="R3:S3"/>
+    <mergeCell ref="N3:O3"/>
+    <mergeCell ref="A1:G1"/>
+    <mergeCell ref="B3:C3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>